<commit_message>
Fix : 몬스터 DB 관련 script 및 excel 수정
</commit_message>
<xml_diff>
--- a/Assets/RawData/MonsterDBSheet.xlsx
+++ b/Assets/RawData/MonsterDBSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\one\Desktop\부트캠프\최종프로젝트 조\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Work\Project_D\Assets\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA47290-06D8-451A-B430-85380D77BB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89827894-BE99-42DB-883F-750E4398BF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3361CD4-ED11-44D2-B071-54130DE34E5B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{B3361CD4-ED11-44D2-B071-54130DE34E5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Monster_Table" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>몬스터 테이블 명세표</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monster_Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>String</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,26 +75,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monster_HP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>몬스터 체력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monster_MP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>몬스터 마나</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster_Atk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Float</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -107,10 +87,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monster_Def</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>몬스터 방어력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -119,38 +95,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monster_Max_Root</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Common_Drop_Per</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>커먼 드랍 확률</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UnCommon_Drop_Per</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>언커먼 드랍 확률</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Rare_Drop_Per</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>레어 드랍 확률</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Unique_Drop_Per</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>유니크 드랍 확률</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -159,34 +115,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster_Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster_HP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster_MP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster_Atk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster_Def</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster_Max_Root</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>스켈레톤 검사</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -224,6 +152,90 @@
   </si>
   <si>
     <t>Unique/2%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 공격 범위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterHp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterAtk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterAtkSpd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterAtkRng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterDef</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterMaxRoot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterRun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterWalk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 걷기 속도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 달리기 속도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_commonDropPer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_uncommonDropPer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_rareDropPer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_uniqueDropPer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterStiff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 피격 후 경직 시간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 공격 속도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -431,7 +443,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -468,29 +480,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -498,6 +492,9 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -513,20 +510,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6157A301-5B48-49C6-8405-9B11D70C9EFF}" name="표1" displayName="표1" ref="A1:K3" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:K3" xr:uid="{6157A301-5B48-49C6-8405-9B11D70C9EFF}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{A31AE133-7C7C-485D-81B2-77F48D81C006}" name="Id"/>
-    <tableColumn id="2" xr3:uid="{24E1B201-12D4-40C3-A0F1-85C510CAF26E}" name="Monster_Name"/>
-    <tableColumn id="3" xr3:uid="{0DA88597-C604-4836-AECA-B8E23FDA3A48}" name="Monster_HP"/>
-    <tableColumn id="4" xr3:uid="{A217850D-FBE5-45DC-B2D9-1E1F82F1B282}" name="Monster_MP"/>
-    <tableColumn id="5" xr3:uid="{4D57E70D-028A-4204-9123-15945C0CA6DD}" name="Monster_Atk"/>
-    <tableColumn id="6" xr3:uid="{E9E55D0C-62B2-4870-BA60-D69CCA36D8D0}" name="Monster_Def"/>
-    <tableColumn id="7" xr3:uid="{5476F9DA-E1CB-4C55-892B-06EFD2F8A434}" name="Monster_Max_Root"/>
-    <tableColumn id="8" xr3:uid="{056BD935-2CCF-4AB9-8506-64213F698BD3}" name="Common_Drop_Per"/>
-    <tableColumn id="9" xr3:uid="{9F9CB5D5-9D60-49DF-8FE5-BD51D0AB5ECE}" name="UnCommon_Drop_Per"/>
-    <tableColumn id="10" xr3:uid="{E7AC8B9E-BD37-4297-96F3-36AD109DD675}" name="Rare_Drop_Per"/>
-    <tableColumn id="11" xr3:uid="{A735305C-8C2A-4E04-AADF-A47713E32BED}" name="Unique_Drop_Per" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6157A301-5B48-49C6-8405-9B11D70C9EFF}" name="표1" displayName="표1" ref="A1:O3" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:O3" xr:uid="{6157A301-5B48-49C6-8405-9B11D70C9EFF}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{A31AE133-7C7C-485D-81B2-77F48D81C006}" name="_id"/>
+    <tableColumn id="2" xr3:uid="{24E1B201-12D4-40C3-A0F1-85C510CAF26E}" name="_monsterName"/>
+    <tableColumn id="3" xr3:uid="{0DA88597-C604-4836-AECA-B8E23FDA3A48}" name="_monsterHp"/>
+    <tableColumn id="4" xr3:uid="{A217850D-FBE5-45DC-B2D9-1E1F82F1B282}" name="_monsterAtk"/>
+    <tableColumn id="5" xr3:uid="{4D57E70D-028A-4204-9123-15945C0CA6DD}" name="_monsterAtkSpd"/>
+    <tableColumn id="13" xr3:uid="{1DF3750D-E20A-4516-9C07-F861D89C3BFC}" name="_monsterAtkRng"/>
+    <tableColumn id="6" xr3:uid="{E9E55D0C-62B2-4870-BA60-D69CCA36D8D0}" name="_monsterDef"/>
+    <tableColumn id="12" xr3:uid="{66BB8D74-A375-46D9-97C0-933F722F71A3}" name="_monsterWalk"/>
+    <tableColumn id="7" xr3:uid="{5476F9DA-E1CB-4C55-892B-06EFD2F8A434}" name="_monsterRun"/>
+    <tableColumn id="8" xr3:uid="{056BD935-2CCF-4AB9-8506-64213F698BD3}" name="_monsterStiff"/>
+    <tableColumn id="9" xr3:uid="{9F9CB5D5-9D60-49DF-8FE5-BD51D0AB5ECE}" name="_monsterMaxRoot"/>
+    <tableColumn id="10" xr3:uid="{E7AC8B9E-BD37-4297-96F3-36AD109DD675}" name="_commonDropPer"/>
+    <tableColumn id="11" xr3:uid="{A735305C-8C2A-4E04-AADF-A47713E32BED}" name="_uncommonDropPer" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{A2FC422F-9B89-450F-96DA-0EAD4BA3E064}" name="_rareDropPer"/>
+    <tableColumn id="15" xr3:uid="{1E43F362-6375-4E5D-BBCD-0E6FD5E3CBC0}" name="_uniqueDropPer"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -849,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C719A-1622-4A1E-8F75-91A245574CF4}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -861,123 +862,159 @@
     <col min="2" max="2" width="19.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>11000001</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>300</v>
       </c>
       <c r="D2">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>0.2</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>11000002</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>150</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <v>0.2</v>
       </c>
       <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J5" s="12"/>
+      <c r="J3">
+        <v>0.2</v>
+      </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -990,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874E174E-728E-416B-9E6C-A7D7D1574A33}">
-  <dimension ref="B1:E14"/>
+  <dimension ref="B1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1029,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -1043,13 +1080,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -1057,13 +1094,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -1071,13 +1108,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
@@ -1085,13 +1122,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
@@ -1099,83 +1136,139 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="7">
-        <v>6</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>28</v>
+      <c r="E14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="7">
+        <v>15</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat : Monster 데이터 적용
</commit_message>
<xml_diff>
--- a/Assets/RawData/MonsterDBSheet.xlsx
+++ b/Assets/RawData/MonsterDBSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Work\Project_D\Assets\RawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Project_D\Assets\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7633A1F-1AA8-4F17-A208-C3722A8F1E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7368B5A-C401-4520-AD87-D45AEFB042B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3361CD4-ED11-44D2-B071-54130DE34E5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3361CD4-ED11-44D2-B071-54130DE34E5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Monster_Table" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>몬스터 테이블 명세표</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -208,6 +208,14 @@
   </si>
   <si>
     <t>_dropId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterChasingRng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_monsterRotationDamping</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -415,7 +423,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -452,9 +460,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -477,9 +482,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6157A301-5B48-49C6-8405-9B11D70C9EFF}" name="표1" displayName="표1" ref="A1:L3" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:L3" xr:uid="{6157A301-5B48-49C6-8405-9B11D70C9EFF}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6157A301-5B48-49C6-8405-9B11D70C9EFF}" name="표1" displayName="표1" ref="A1:N3" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:N3" xr:uid="{6157A301-5B48-49C6-8405-9B11D70C9EFF}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{A31AE133-7C7C-485D-81B2-77F48D81C006}" name="_id"/>
     <tableColumn id="2" xr3:uid="{24E1B201-12D4-40C3-A0F1-85C510CAF26E}" name="_monsterName"/>
     <tableColumn id="3" xr3:uid="{0DA88597-C604-4836-AECA-B8E23FDA3A48}" name="_monsterHp"/>
@@ -492,6 +497,8 @@
     <tableColumn id="8" xr3:uid="{056BD935-2CCF-4AB9-8506-64213F698BD3}" name="_monsterStiff"/>
     <tableColumn id="9" xr3:uid="{9F9CB5D5-9D60-49DF-8FE5-BD51D0AB5ECE}" name="_monsterMaxRoot"/>
     <tableColumn id="10" xr3:uid="{E7AC8B9E-BD37-4297-96F3-36AD109DD675}" name="_dropId"/>
+    <tableColumn id="11" xr3:uid="{071CCEA1-66FE-4FCC-81B0-10CDF197FADB}" name="_monsterChasingRng"/>
+    <tableColumn id="14" xr3:uid="{7E9F1C1B-D1BB-4E38-A6A6-E8F49E247D4C}" name="_monsterRotationDamping"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -814,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9C719A-1622-4A1E-8F75-91A245574CF4}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -839,7 +846,7 @@
     <col min="15" max="15" width="18.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -876,11 +883,14 @@
       <c r="L1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>11000001</v>
       </c>
@@ -917,8 +927,14 @@
       <c r="L2">
         <v>10000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>11000002</v>
       </c>
@@ -954,6 +970,12 @@
       </c>
       <c r="L3">
         <v>10000002</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>